<commit_message>
stu upload function have problem in foreign_stu 學籍狀態
</commit_message>
<xml_diff>
--- a/public/Excel_example/stu/foreign_stu.xlsx
+++ b/public/Excel_example/stu/foreign_stu.xlsx
@@ -524,7 +524,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -532,7 +532,13 @@
   <cols>
     <col min="1" max="1" width="16.625" customWidth="1"/>
     <col min="2" max="2" width="17.25" customWidth="1"/>
+    <col min="4" max="4" width="10.625" customWidth="1"/>
     <col min="6" max="6" width="27.25" customWidth="1"/>
+    <col min="7" max="7" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="11.875" customWidth="1"/>
+    <col min="10" max="10" width="11.625" customWidth="1"/>
+    <col min="11" max="11" width="12.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>